<commit_message>
Full pt names sheet
</commit_message>
<xml_diff>
--- a/B3 pt names.xlsx
+++ b/B3 pt names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujia1998/Desktop/Work/Reading Center/B3VF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45CEA3B-7927-DF4C-A044-D5F97AD03FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9485FF12-9EB3-A647-B02C-153A84FC4DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4760" yWindow="620" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="196">
   <si>
     <t>Last Name</t>
   </si>
@@ -486,23 +486,152 @@
     <t>Rachel</t>
   </si>
   <si>
-    <t xml:space="preserve">Patient ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Study ID </t>
-  </si>
-  <si>
     <t>Patient Last Name</t>
   </si>
   <si>
     <t>Patient First Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>CUNAD004</t>
+  </si>
+  <si>
+    <t>CUNAD008</t>
+  </si>
+  <si>
+    <t>CUNAD010</t>
+  </si>
+  <si>
+    <t>CUNAD017</t>
+  </si>
+  <si>
+    <t>CUNAD018</t>
+  </si>
+  <si>
+    <t>CUNAD020</t>
+  </si>
+  <si>
+    <t>CUNAD026</t>
+  </si>
+  <si>
+    <t>CUNAD027</t>
+  </si>
+  <si>
+    <t>CUNAD033</t>
+  </si>
+  <si>
+    <t>CUNAD037</t>
+  </si>
+  <si>
+    <t>CUNAD040</t>
+  </si>
+  <si>
+    <t>CUNAD045</t>
+  </si>
+  <si>
+    <t>CUNAD049</t>
+  </si>
+  <si>
+    <t>CUNAD055</t>
+  </si>
+  <si>
+    <t>CUNAD059</t>
+  </si>
+  <si>
+    <t>CUNAD102</t>
+  </si>
+  <si>
+    <t>Cohen</t>
+  </si>
+  <si>
+    <t>Marumoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renol </t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Trotz</t>
+  </si>
+  <si>
+    <t>Zeigler</t>
+  </si>
+  <si>
+    <t>Tao</t>
+  </si>
+  <si>
+    <t>Rubinson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wintner </t>
+  </si>
+  <si>
+    <t>Applewhaite</t>
+  </si>
+  <si>
+    <t>Sobel</t>
+  </si>
+  <si>
+    <t>Rayman</t>
+  </si>
+  <si>
+    <t>Feldman</t>
+  </si>
+  <si>
+    <t>Berkvist</t>
+  </si>
+  <si>
+    <t>Seo</t>
+  </si>
+  <si>
+    <t>Terry</t>
+  </si>
+  <si>
+    <t>Claire</t>
+  </si>
+  <si>
+    <t>Lominy</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Joan</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Rhonda</t>
+  </si>
+  <si>
+    <t>Allan</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>Anita</t>
+  </si>
+  <si>
+    <t>Henrietta</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,16 +661,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -679,115 +798,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b val="0"/>
@@ -824,10 +855,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1093,19 +1120,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK62"/>
+  <dimension ref="A1:AK66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.1640625" style="2"/>
@@ -1113,22 +1140,22 @@
   <sheetData>
     <row r="1" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1223,14 +1250,14 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f t="shared" ref="C3:C50" si="0" xml:space="preserve"> UPPER(B3)</f>
+        <f t="shared" ref="C3:C66" si="0" xml:space="preserve"> UPPER(B3)</f>
         <v>CHOWDHURY</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="str">
-        <f t="shared" ref="E3:E50" si="1">UPPER(D3)</f>
+        <f t="shared" ref="E3:E66" si="1">UPPER(D3)</f>
         <v>SUBHABRATA</v>
       </c>
       <c r="F3" s="15">
@@ -1291,25 +1318,25 @@
       </c>
     </row>
     <row r="5" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
+      <c r="A5" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>LEVINE</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>COHEN</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LAURIE</v>
-      </c>
-      <c r="F5" s="15">
-        <v>1007655201</v>
+        <v>TERRY</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1001865737</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1345,135 +1372,135 @@
     </row>
     <row r="6" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>TUNIOLI</v>
+        <v>LEVINE</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>CARLO</v>
+        <v>LAURIE</v>
       </c>
       <c r="F6" s="15">
-        <v>1101992349</v>
+        <v>1007655201</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>MUNRO</v>
+        <v>TUNIOLI</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>HELEN</v>
-      </c>
-      <c r="F7" s="14">
-        <v>1000400996</v>
+        <v>CARLO</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1101992349</v>
       </c>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>O'MALLEY</v>
+        <v>MUNRO</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>JUDY</v>
-      </c>
-      <c r="F8" s="15">
-        <v>1201621306</v>
+        <v>HELEN</v>
+      </c>
+      <c r="F8" s="14">
+        <v>1000400996</v>
       </c>
     </row>
     <row r="9" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
+      <c r="A9" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>CALLOWAY</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>MARUMOTO</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DEBRA</v>
-      </c>
-      <c r="F9" s="15">
-        <v>1102443341</v>
+        <v>CLAIRE</v>
+      </c>
+      <c r="F9" s="20">
+        <v>1203348863</v>
       </c>
     </row>
     <row r="10" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>KANOWITH</v>
+        <v>O'MALLEY</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DANIEL</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1203261574</v>
+        <v>JUDY</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1201621306</v>
       </c>
     </row>
     <row r="11" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
+      <c r="A11" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GROLLMAN</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v xml:space="preserve">RENOL </v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ANNETTE</v>
-      </c>
-      <c r="F11" s="15">
-        <v>1005006415</v>
+        <v>LOMINY</v>
+      </c>
+      <c r="F11" s="20">
+        <v>1101635616</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1509,46 +1536,46 @@
     </row>
     <row r="12" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>KURZ</v>
+        <v>CALLOWAY</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">STEVEN </v>
-      </c>
-      <c r="F12" s="14">
-        <v>1000030971</v>
+        <v>DEBRA</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1102443341</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>36</v>
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>NASHEL</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>37</v>
+        <v>KANOWITH</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>SUSAN</v>
-      </c>
-      <c r="F13" s="16">
-        <v>1004547291</v>
+        <v>DANIEL</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1203261574</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1584,24 +1611,24 @@
     </row>
     <row r="14" spans="1:37" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">WOODLEY </v>
+        <v>GROLLMAN</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KEVIN</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1008603212</v>
+        <v>ANNETTE</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1005006415</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1637,90 +1664,90 @@
     </row>
     <row r="15" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>JOHN</v>
+        <v>KURZ</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DENNIS K</v>
-      </c>
-      <c r="F15" s="15">
-        <v>1005204161</v>
+        <v xml:space="preserve">STEVEN </v>
+      </c>
+      <c r="F15" s="14">
+        <v>1000030971</v>
       </c>
     </row>
     <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>45</v>
+      <c r="A16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>LEVY</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>NASHEL</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>YAEL V</v>
-      </c>
-      <c r="F16" s="14">
-        <v>1008970046</v>
+        <v>SUSAN</v>
+      </c>
+      <c r="F16" s="16">
+        <v>1004547291</v>
       </c>
     </row>
     <row r="17" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GLOGOWER</v>
+        <v xml:space="preserve">WOODLEY </v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">GARY </v>
-      </c>
-      <c r="F17" s="15">
-        <v>1002137827</v>
+        <v>KEVIN</v>
+      </c>
+      <c r="F17" s="14">
+        <v>1008603212</v>
       </c>
     </row>
     <row r="18" spans="1:37" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>51</v>
+      <c r="A18" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>KRUGER</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>52</v>
+        <v>SILVER</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ROBERT</v>
-      </c>
-      <c r="F18" s="14">
-        <v>1006803388</v>
+        <v>JONATHAN</v>
+      </c>
+      <c r="F18" s="20">
+        <v>1000406553</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1755,47 +1782,47 @@
       <c r="AK18" s="2"/>
     </row>
     <row r="19" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>54</v>
+      <c r="A19" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>172</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>RETREY</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>TROTZ</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MARCIA</v>
-      </c>
-      <c r="F19" s="15">
-        <v>1002759255</v>
+        <v>JOAN</v>
+      </c>
+      <c r="F19" s="21">
+        <v>1400012385</v>
       </c>
     </row>
     <row r="20" spans="1:37" s="10" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>SMART</v>
+        <v>JOHN</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ANTOINETTE</v>
+        <v>DENNIS K</v>
       </c>
       <c r="F20" s="15">
-        <v>1003076205</v>
+        <v>1005204161</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1830,25 +1857,25 @@
       <c r="AK20" s="2"/>
     </row>
     <row r="21" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>60</v>
+      <c r="A21" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ABELS </v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>61</v>
+        <v>ZEIGLER</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KATHLEEN</v>
-      </c>
-      <c r="F21" s="15">
-        <v>1400990930</v>
+        <v>FRED</v>
+      </c>
+      <c r="F21" s="21">
+        <v>1200547700</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1883,25 +1910,25 @@
       <c r="AK21" s="2"/>
     </row>
     <row r="22" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>63</v>
+      <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>MORAWEK</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>64</v>
+        <v>LEVY</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>GRACEANN</v>
-      </c>
-      <c r="F22" s="17">
-        <v>1101725996</v>
+        <v>YAEL V</v>
+      </c>
+      <c r="F22" s="14">
+        <v>1008970046</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1937,68 +1964,68 @@
     </row>
     <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>LAROSE</v>
+        <v>GLOGOWER</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>IAN</v>
+        <v xml:space="preserve">GARY </v>
       </c>
       <c r="F23" s="15">
-        <v>1100340217</v>
+        <v>1002137827</v>
       </c>
     </row>
     <row r="24" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>BRODER</v>
+        <v>KRUGER</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>JOSHUA</v>
+        <v>ROBERT</v>
       </c>
       <c r="F24" s="14">
-        <v>1006919645</v>
+        <v>1006803388</v>
       </c>
     </row>
     <row r="25" spans="1:37" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>HSIEH</v>
+        <v>RETREY</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>CHRISTINE</v>
+        <v>MARCIA</v>
       </c>
       <c r="F25" s="15">
-        <v>1010234467</v>
+        <v>1002759255</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2034,46 +2061,46 @@
     </row>
     <row r="26" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>SHETH</v>
+        <v>SMART</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>RUPESH</v>
+        <v>ANTOINETTE</v>
       </c>
       <c r="F26" s="15">
-        <v>1400833342</v>
+        <v>1003076205</v>
       </c>
     </row>
     <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>78</v>
+      <c r="A27" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>174</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>GEIST</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>79</v>
+        <v>TAO</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>CAROL</v>
-      </c>
-      <c r="F27" s="16">
-        <v>1002525369</v>
+        <v>JONATHAN</v>
+      </c>
+      <c r="F27" s="21">
+        <v>1101634399</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -2108,69 +2135,69 @@
       <c r="AK27" s="10"/>
     </row>
     <row r="28" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>81</v>
+      <c r="A28" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>175</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>OH</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>82</v>
+        <v>RUBINSON</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>SUN YOUNG</v>
-      </c>
-      <c r="F28" s="16">
-        <v>1102500564</v>
+        <v>RHONDA</v>
+      </c>
+      <c r="F28" s="21">
+        <v>1008949437</v>
       </c>
     </row>
     <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>LAM</v>
+        <v xml:space="preserve">ABELS </v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">TAN </v>
-      </c>
-      <c r="F29" s="14">
-        <v>1006322385</v>
+        <v>KATHLEEN</v>
+      </c>
+      <c r="F29" s="15">
+        <v>1400990930</v>
       </c>
     </row>
     <row r="30" spans="1:37" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>87</v>
+      <c r="A30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>BERTALAN</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>88</v>
+        <v>MORAWEK</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MARGRET S</v>
-      </c>
-      <c r="F30" s="14">
-        <v>1007579054</v>
+        <v>GRACEANN</v>
+      </c>
+      <c r="F30" s="17">
+        <v>1101725996</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -2206,68 +2233,68 @@
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>MARTIN</v>
+        <v>LAROSE</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">ROBIN </v>
-      </c>
-      <c r="F31" s="14">
-        <v>1004589159</v>
+        <v>IAN</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1100340217</v>
       </c>
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>PULEIO</v>
+        <v>BRODER</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ANNMARIE</v>
+        <v>JOSHUA</v>
       </c>
       <c r="F32" s="14">
-        <v>1400111785</v>
+        <v>1006919645</v>
       </c>
     </row>
     <row r="33" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="A33" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>96</v>
+      <c r="A33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>RUBIN</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>97</v>
+        <v>HSIEH</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="E33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">KAREN </v>
-      </c>
-      <c r="F33" s="16">
-        <v>1203529686</v>
+        <v>CHRISTINE</v>
+      </c>
+      <c r="F33" s="15">
+        <v>1010234467</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
@@ -2302,25 +2329,25 @@
       <c r="AK33" s="10"/>
     </row>
     <row r="34" spans="1:37" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>99</v>
+      <c r="A34" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="C34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ABRAMOWITZ</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>100</v>
+        <v>LEVINE</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="E34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>AVRAM</v>
-      </c>
-      <c r="F34" s="14">
-        <v>1009615947</v>
+        <v>ALLAN</v>
+      </c>
+      <c r="F34" s="22">
+        <v>1004225323</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2355,135 +2382,135 @@
       <c r="AK34" s="2"/>
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>102</v>
+      <c r="A35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>FORSMAN</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>103</v>
+        <v>SHETH</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KARL</v>
-      </c>
-      <c r="F35" s="14">
-        <v>1400389901</v>
+        <v>RUPESH</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1400833342</v>
       </c>
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>105</v>
+      <c r="A36" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>IBANEZ</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>106</v>
+        <v>GEIST</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>ELIZABETH</v>
-      </c>
-      <c r="F36" s="14">
-        <v>1004720906</v>
+        <v>CAROL</v>
+      </c>
+      <c r="F36" s="16">
+        <v>1002525369</v>
       </c>
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>108</v>
+      <c r="A37" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>LOUIS</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>109</v>
+        <v>OH</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>KENNETH</v>
-      </c>
-      <c r="F37" s="14">
-        <v>1101738414</v>
+        <v>SUN YOUNG</v>
+      </c>
+      <c r="F37" s="16">
+        <v>1102500564</v>
       </c>
     </row>
     <row r="38" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>111</v>
+      <c r="A38" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>KENNEY</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>112</v>
+        <v xml:space="preserve">WINTNER </v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="E38" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>JAMES</v>
-      </c>
-      <c r="F38" s="14">
-        <v>1101633005</v>
+        <v>MARK</v>
+      </c>
+      <c r="F38" s="21">
+        <v>1010621689</v>
       </c>
     </row>
     <row r="39" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>114</v>
+        <v>83</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>BARQUIN</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>115</v>
+        <v>LAM</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="E39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>JOSE</v>
+        <v xml:space="preserve">TAN </v>
       </c>
       <c r="F39" s="14">
-        <v>1101640191</v>
+        <v>1006322385</v>
       </c>
     </row>
     <row r="40" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>SIGMAN</v>
+        <v>BERTALAN</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="E40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MICHELLE E</v>
+        <v>MARGRET S</v>
       </c>
       <c r="F40" s="14">
-        <v>1201237092</v>
+        <v>1007579054</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2518,91 +2545,91 @@
       <c r="AK40" s="2"/>
     </row>
     <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>120</v>
+      <c r="A41" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>WILKS</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>121</v>
+        <v>APPLEWHAITE</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>192</v>
       </c>
       <c r="E41" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>STEPHEN</v>
-      </c>
-      <c r="F41" s="14">
-        <v>1101632952</v>
+        <v>FRANCES</v>
+      </c>
+      <c r="F41" s="21">
+        <v>1007179151</v>
       </c>
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>FANOUS</v>
+        <v>MARTIN</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="E42" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>MARY</v>
+        <v xml:space="preserve">ROBIN </v>
       </c>
       <c r="F42" s="14">
-        <v>1400457249</v>
+        <v>1004589159</v>
       </c>
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="C43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>VENK</v>
+        <v>PULEIO</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="E43" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>RONALD</v>
+        <v>ANNMARIE</v>
       </c>
       <c r="F43" s="14">
-        <v>1003897651</v>
+        <v>1400111785</v>
       </c>
     </row>
     <row r="44" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A44" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>129</v>
+      <c r="A44" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="C44" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">GANGOLF </v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>130</v>
+        <v>RUBIN</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="E44" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">DREW </v>
-      </c>
-      <c r="F44" s="14">
-        <v>1100780728</v>
+        <v xml:space="preserve">KAREN </v>
+      </c>
+      <c r="F44" s="16">
+        <v>1203529686</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2638,68 +2665,68 @@
     </row>
     <row r="45" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="C45" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>HODGKIN</v>
+        <v>ABRAMOWITZ</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="E45" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>CARTER D</v>
+        <v>AVRAM</v>
       </c>
       <c r="F45" s="14">
-        <v>1010439237</v>
+        <v>1009615947</v>
       </c>
     </row>
     <row r="46" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="A46" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>135</v>
+      <c r="A46" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>178</v>
       </c>
       <c r="C46" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ROCHE</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>136</v>
+        <v>SOBEL</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="E46" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">CHRISTOPHER </v>
-      </c>
-      <c r="F46" s="14">
-        <v>1007125987</v>
+        <v>SUSAN</v>
+      </c>
+      <c r="F46" s="21">
+        <v>1401023875</v>
       </c>
     </row>
     <row r="47" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="C47" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">ZAMORA </v>
+        <v>FORSMAN</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="E47" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>CARLOS</v>
+        <v>KARL</v>
       </c>
       <c r="F47" s="14">
-        <v>1203533770</v>
+        <v>1400389901</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2734,47 +2761,47 @@
       <c r="AK47" s="2"/>
     </row>
     <row r="48" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>141</v>
+      <c r="A48" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C48" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>RANDALL</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>142</v>
+        <v>IBANEZ</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="E48" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>THEODORE</v>
-      </c>
-      <c r="F48" s="19">
-        <v>1006412449</v>
+        <v>ELIZABETH</v>
+      </c>
+      <c r="F48" s="14">
+        <v>1004720906</v>
       </c>
     </row>
     <row r="49" spans="1:37" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A49" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>144</v>
+      <c r="A49" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C49" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>HINZMANN</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>145</v>
+        <v>LOUIS</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="E49" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>HILARY</v>
-      </c>
-      <c r="F49" s="16">
-        <v>1007372951</v>
+        <v>KENNETH</v>
+      </c>
+      <c r="F49" s="14">
+        <v>1101738414</v>
       </c>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -2809,68 +2836,382 @@
       <c r="AK49" s="10"/>
     </row>
     <row r="50" spans="1:37" s="10" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>RAYMAN</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E50" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>ANITA</v>
+      </c>
+      <c r="F50" s="23">
+        <v>1100069305</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>KENNEY</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>JAMES</v>
+      </c>
+      <c r="F51" s="14">
+        <v>1101633005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>BARQUIN</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>JOSE</v>
+      </c>
+      <c r="F52" s="14">
+        <v>1101640191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A53" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>SIGMAN</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>MICHELLE E</v>
+      </c>
+      <c r="F53" s="14">
+        <v>1201237092</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A54" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>WILKS</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>STEPHEN</v>
+      </c>
+      <c r="F54" s="14">
+        <v>1101632952</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>FANOUS</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E55" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>MARY</v>
+      </c>
+      <c r="F55" s="14">
+        <v>1400457249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A56" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>FELDMAN</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E56" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>HENRIETTA</v>
+      </c>
+      <c r="F56" s="21">
+        <v>1101635600</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A57" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>VENK</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E57" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>RONALD</v>
+      </c>
+      <c r="F57" s="14">
+        <v>1003897651</v>
+      </c>
+    </row>
+    <row r="58" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A58" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">GANGOLF </v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">DREW </v>
+      </c>
+      <c r="F58" s="14">
+        <v>1100780728</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A59" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>HODGKIN</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E59" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>CARTER D</v>
+      </c>
+      <c r="F59" s="14">
+        <v>1010439237</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A60" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C60" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>BERKVIST</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E60" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>CAROL</v>
+      </c>
+      <c r="F60" s="21">
+        <v>1005732833</v>
+      </c>
+    </row>
+    <row r="61" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A61" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>ROCHE</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E61" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">CHRISTOPHER </v>
+      </c>
+      <c r="F61" s="14">
+        <v>1007125987</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37" ht="14" x14ac:dyDescent="0.15">
+      <c r="A62" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ZAMORA </v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>CARLOS</v>
+      </c>
+      <c r="F62" s="14">
+        <v>1203533770</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>RANDALL</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E63" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>THEODORE</v>
+      </c>
+      <c r="F63" s="18">
+        <v>1006412449</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>HINZMANN</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>HILARY</v>
+      </c>
+      <c r="F64" s="16">
+        <v>1007372951</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>SEO</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E65" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>HILARY</v>
+      </c>
+      <c r="F65" s="22">
+        <v>1400282808</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B66" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="2" t="str">
+      <c r="C66" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MOHAMMED</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D66" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E50" s="2" t="str">
+      <c r="E66" s="2" t="str">
         <f t="shared" si="1"/>
         <v>RACHEL</v>
       </c>
-      <c r="F50" s="16">
+      <c r="F66" s="16">
         <v>1000172439</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="22"/>
-    </row>
-    <row r="52" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="22"/>
-    </row>
-    <row r="53" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="23"/>
-    </row>
-    <row r="54" spans="1:37" ht="16" x14ac:dyDescent="0.2">
-      <c r="E54" s="22"/>
-      <c r="F54" s="18"/>
-    </row>
-    <row r="55" spans="1:37" ht="16" x14ac:dyDescent="0.2">
-      <c r="E55" s="22"/>
-      <c r="F55" s="18"/>
-    </row>
-    <row r="56" spans="1:37" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="57" spans="1:37" ht="14" x14ac:dyDescent="0.15">
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="22"/>
-    </row>
-    <row r="58" spans="1:37" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="59" spans="1:37" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="60" spans="1:37" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="61" spans="1:37" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="62" spans="1:37" ht="14" x14ac:dyDescent="0.15"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:AK174">
-    <sortCondition sortBy="fontColor" ref="A1:A174" dxfId="4"/>
+    <sortCondition sortBy="fontColor" ref="A1:A174" dxfId="0"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2903,15 +3244,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA5A02F4E9BED54B8CA066912D18D8C3" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a3d71277f3013e2869e7a4224cf671c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b81f02b7-5000-41f9-adda-eb34efa280f9" xmlns:ns3="8ef98a62-a8be-4b29-8c57-646a407091ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3158e8f89e4d5ae1acf5e619439050f5" ns2:_="" ns3:_="">
     <xsd:import namespace="b81f02b7-5000-41f9-adda-eb34efa280f9"/>
@@ -3160,6 +3492,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACA91056-72B8-4F8B-9836-59FCFB05A012}">
   <ds:schemaRefs>
@@ -3172,14 +3513,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66370FCB-667C-4A2A-B16F-331C98464747}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E4AEFCA-AF65-4726-8D16-E716A20DBCB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3196,4 +3529,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66370FCB-667C-4A2A-B16F-331C98464747}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Full pt names list
</commit_message>
<xml_diff>
--- a/B3 pt names.xlsx
+++ b/B3 pt names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujia1998/Desktop/Work/Reading Center/B3VF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD20D1CA-0579-D340-A516-10E4136075D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1A6C7E-6CEB-9F49-B24E-58BE89049812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11680" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master List" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="197">
   <si>
     <t>Last Name</t>
   </si>
@@ -102,12 +102,6 @@
     <t>CUNAD009</t>
   </si>
   <si>
-    <t>O'Malley</t>
-  </si>
-  <si>
-    <t>Judy</t>
-  </si>
-  <si>
     <t>CUNAD011</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>John</t>
   </si>
   <si>
-    <t>Dennis K</t>
-  </si>
-  <si>
     <t>CUNAD021</t>
   </si>
   <si>
@@ -228,9 +219,6 @@
     <t>Morawek</t>
   </si>
   <si>
-    <t>Graceann</t>
-  </si>
-  <si>
     <t>CUNAD030</t>
   </si>
   <si>
@@ -282,9 +270,6 @@
     <t>Oh</t>
   </si>
   <si>
-    <t>Sun Young</t>
-  </si>
-  <si>
     <t>CUNAD038</t>
   </si>
   <si>
@@ -330,9 +315,6 @@
     <t>CUNAD044</t>
   </si>
   <si>
-    <t>Abramowitz</t>
-  </si>
-  <si>
     <t>Avram</t>
   </si>
   <si>
@@ -390,9 +372,6 @@
     <t>CUNAD053</t>
   </si>
   <si>
-    <t>Wilks</t>
-  </si>
-  <si>
     <t>Stephen</t>
   </si>
   <si>
@@ -420,9 +399,6 @@
     <t xml:space="preserve">Gangolf </t>
   </si>
   <si>
-    <t xml:space="preserve">Drew </t>
-  </si>
-  <si>
     <t>CUNAD058</t>
   </si>
   <si>
@@ -537,9 +513,6 @@
     <t>Marumoto</t>
   </si>
   <si>
-    <t xml:space="preserve">Renol </t>
-  </si>
-  <si>
     <t>Silver</t>
   </si>
   <si>
@@ -576,9 +549,6 @@
     <t>Seo</t>
   </si>
   <si>
-    <t>Terry</t>
-  </si>
-  <si>
     <t>Claire</t>
   </si>
   <si>
@@ -624,7 +594,40 @@
     <t>Carter</t>
   </si>
   <si>
-    <t xml:space="preserve">Margret </t>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Carol M</t>
+  </si>
+  <si>
+    <t>Graceann V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrew </t>
+  </si>
+  <si>
+    <t>Abramowitz MD</t>
+  </si>
+  <si>
+    <t>Judith</t>
+  </si>
+  <si>
+    <t>OMalley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margaret </t>
+  </si>
+  <si>
+    <t>Renol</t>
+  </si>
+  <si>
+    <t>Wilk</t>
+  </si>
+  <si>
+    <t>Teresa</t>
+  </si>
+  <si>
+    <t>Sun</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1127,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1140,22 +1143,22 @@
   <sheetData>
     <row r="1" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1319,21 +1322,21 @@
     </row>
     <row r="5" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>COHEN</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>TERRY</v>
+        <v>TERESA</v>
       </c>
       <c r="F5" s="20">
         <v>1001865737</v>
@@ -1439,17 +1442,17 @@
     </row>
     <row r="9" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MARUMOTO</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1464,18 +1467,18 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>O'MALLEY</v>
+        <f xml:space="preserve"> UPPER(B10)</f>
+        <v>OMALLEY</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="E10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>JUDY</v>
+        <f>UPPER(D10)</f>
+        <v>JUDITH</v>
       </c>
       <c r="F10" s="15">
         <v>1201621306</v>
@@ -1483,21 +1486,21 @@
     </row>
     <row r="11" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">RENOL </v>
+        <v>LOMINY</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LOMINY</v>
+        <v>RENOL</v>
       </c>
       <c r="F11" s="20">
         <v>1101635616</v>
@@ -1536,17 +1539,17 @@
     </row>
     <row r="12" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>CALLOWAY</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>CALLOWAY</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1558,17 +1561,17 @@
     </row>
     <row r="13" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>KANOWITH</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>KANOWITH</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1611,17 +1614,17 @@
     </row>
     <row r="14" spans="1:37" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>GROLLMAN</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>GROLLMAN</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1664,17 +1667,17 @@
     </row>
     <row r="15" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>KURZ</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>KURZ</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1686,17 +1689,17 @@
     </row>
     <row r="16" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>NASHEL</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>NASHEL</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1708,17 +1711,17 @@
     </row>
     <row r="17" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">WOODLEY </v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">WOODLEY </v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1730,17 +1733,17 @@
     </row>
     <row r="18" spans="1:37" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>SILVER</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1783,17 +1786,17 @@
     </row>
     <row r="19" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>TROTZ</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1805,21 +1808,21 @@
     </row>
     <row r="20" spans="1:37" s="10" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>JOHN</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>185</v>
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>DENNIS K</v>
+        <v>DENNIS</v>
       </c>
       <c r="F20" s="15">
         <v>1005204161</v>
@@ -1858,17 +1861,17 @@
     </row>
     <row r="21" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ZEIGLER</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1911,17 +1914,17 @@
     </row>
     <row r="22" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>LEVY</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="E22" s="2" t="str">
         <f>UPPER(D22)</f>
@@ -1964,17 +1967,17 @@
     </row>
     <row r="23" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GLOGOWER</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E23" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1986,17 +1989,17 @@
     </row>
     <row r="24" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>KRUGER</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E24" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2008,17 +2011,17 @@
     </row>
     <row r="25" spans="1:37" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>RETREY</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E25" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2061,17 +2064,17 @@
     </row>
     <row r="26" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>SMART</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2083,17 +2086,17 @@
     </row>
     <row r="27" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>TAO</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2136,17 +2139,17 @@
     </row>
     <row r="28" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>RUBINSON</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2158,17 +2161,17 @@
     </row>
     <row r="29" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ABELS </v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2180,21 +2183,21 @@
     </row>
     <row r="30" spans="1:37" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MORAWEK</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>63</v>
+        <v>187</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>GRACEANN</v>
+        <v>GRACEANN V</v>
       </c>
       <c r="F30" s="17">
         <v>1101725996</v>
@@ -2233,17 +2236,17 @@
     </row>
     <row r="31" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>LAROSE</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2255,17 +2258,17 @@
     </row>
     <row r="32" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>BRODER</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2277,17 +2280,17 @@
     </row>
     <row r="33" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>HSIEH</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E33" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2330,7 +2333,7 @@
     </row>
     <row r="34" spans="1:37" s="13" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="11" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>12</v>
@@ -2340,7 +2343,7 @@
         <v>LEVINE</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E34" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2383,17 +2386,17 @@
     </row>
     <row r="35" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>SHETH</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E35" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2405,17 +2408,17 @@
     </row>
     <row r="36" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>GEIST</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2427,21 +2430,21 @@
     </row>
     <row r="37" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>OH</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>81</v>
+        <v>196</v>
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>SUN YOUNG</v>
+        <v>SUN</v>
       </c>
       <c r="F37" s="16">
         <v>1102500564</v>
@@ -2449,17 +2452,17 @@
     </row>
     <row r="38" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C38" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">WINTNER </v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="E38" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2471,17 +2474,17 @@
     </row>
     <row r="39" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>LAM</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E39" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2493,21 +2496,21 @@
     </row>
     <row r="40" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>BERTALAN</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">MARGRET </v>
+        <v xml:space="preserve">MARGARET </v>
       </c>
       <c r="F40" s="14">
         <v>1007579054</v>
@@ -2546,17 +2549,17 @@
     </row>
     <row r="41" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C41" s="2" t="str">
         <f t="shared" si="0"/>
         <v>APPLEWHAITE</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E41" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2568,17 +2571,17 @@
     </row>
     <row r="42" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MARTIN</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E42" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2590,17 +2593,17 @@
     </row>
     <row r="43" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>PULEIO</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E43" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2612,17 +2615,17 @@
     </row>
     <row r="44" spans="1:37" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="10" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>RUBIN</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E44" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2665,17 +2668,17 @@
     </row>
     <row r="45" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="C45" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>ABRAMOWITZ</v>
+        <v>ABRAMOWITZ MD</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E45" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2687,17 +2690,17 @@
     </row>
     <row r="46" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C46" s="2" t="str">
         <f t="shared" si="0"/>
         <v>SOBEL</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E46" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2709,17 +2712,17 @@
     </row>
     <row r="47" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C47" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FORSMAN</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E47" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2762,17 +2765,17 @@
     </row>
     <row r="48" spans="1:37" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C48" s="2" t="str">
         <f t="shared" si="0"/>
         <v>IBANEZ</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E48" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2784,17 +2787,17 @@
     </row>
     <row r="49" spans="1:37" s="11" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>LOUIS</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E49" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2837,17 +2840,17 @@
     </row>
     <row r="50" spans="1:37" s="10" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="13" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C50" s="2" t="str">
         <f t="shared" si="0"/>
         <v>RAYMAN</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E50" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2859,17 +2862,17 @@
     </row>
     <row r="51" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>KENNEY</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E51" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2881,17 +2884,17 @@
     </row>
     <row r="52" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>BARQUIN</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E52" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2903,17 +2906,17 @@
     </row>
     <row r="53" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>SIGMAN</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="E53" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2925,17 +2928,17 @@
     </row>
     <row r="54" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>117</v>
+        <v>194</v>
       </c>
       <c r="C54" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>WILKS</v>
+        <v>WILK</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E54" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2947,17 +2950,17 @@
     </row>
     <row r="55" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C55" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FANOUS</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E55" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2969,17 +2972,17 @@
     </row>
     <row r="56" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C56" s="2" t="str">
         <f t="shared" si="0"/>
         <v>FELDMAN</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E56" s="2" t="str">
         <f t="shared" si="1"/>
@@ -2991,17 +2994,17 @@
     </row>
     <row r="57" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C57" s="2" t="str">
         <f t="shared" si="0"/>
         <v>VENK</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E57" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3013,21 +3016,21 @@
     </row>
     <row r="58" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C58" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">GANGOLF </v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="E58" s="2" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">DREW </v>
+        <v xml:space="preserve">ANDREW </v>
       </c>
       <c r="F58" s="14">
         <v>1100780728</v>
@@ -3035,17 +3038,17 @@
     </row>
     <row r="59" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C59" s="2" t="str">
         <f t="shared" si="0"/>
         <v>HODGKIN</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E59" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3057,21 +3060,21 @@
     </row>
     <row r="60" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C60" s="2" t="str">
         <f t="shared" si="0"/>
         <v>BERKVIST</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="E60" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>CAROL</v>
+        <v>CAROL M</v>
       </c>
       <c r="F60" s="21">
         <v>1005732833</v>
@@ -3079,17 +3082,17 @@
     </row>
     <row r="61" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C61" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROCHE</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E61" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3101,17 +3104,17 @@
     </row>
     <row r="62" spans="1:37" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C62" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">ZAMORA </v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E62" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3123,17 +3126,17 @@
     </row>
     <row r="63" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C63" s="2" t="str">
         <f t="shared" si="0"/>
         <v>RANDALL</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E63" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3145,17 +3148,17 @@
     </row>
     <row r="64" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C64" s="2" t="str">
         <f t="shared" si="0"/>
         <v>HINZMANN</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E64" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3167,17 +3170,17 @@
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="11" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C65" s="2" t="str">
         <f t="shared" si="0"/>
         <v>SEO</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E65" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3189,17 +3192,17 @@
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="10" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C66" s="2" t="str">
         <f t="shared" si="0"/>
         <v>MOHAMMED</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E66" s="2" t="str">
         <f t="shared" si="1"/>

</xml_diff>